<commit_message>
updates to  searchparam url and id
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/client.xlsx
+++ b/input/resources-spreadsheet/client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Argo-PL/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2340E2-F4C3-644B-BA4F-FCFD35FE61A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55109704-AFC1-A94A-B7AE-453BC6B910AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-720" windowWidth="25600" windowHeight="20480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="-720" windowWidth="25600" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -358,9 +358,6 @@
     <t>profile_conf</t>
   </si>
   <si>
-    <t>0.2.0</t>
-  </si>
-  <si>
     <t>transaction</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>Argonaut</t>
   </si>
   <si>
-    <t xml:space="preserve"> http://www.fhir.org/guides/argonaut/patient-list/</t>
-  </si>
-  <si>
     <t>Argonaut Project</t>
   </si>
   <si>
@@ -416,14 +410,6 @@
   </si>
   <si>
     <t>doc_Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This CapabilityStatement outlines the conformance requirements and expectations for the Argonaut User Facing Patient List **Client applications**.  It identifies the specific profiles and RESTful transactions for  requesting user facing patient list data from an EHR using the Argonaut User Facing Patient List API.  This includes the following interactions:
-1. Discovery of User Facing Patient Lists
-2. Fetching User Facing Patient Lists
-3. Fetching Additional Data about each Patient in a User Facing Patient Lists
-This is a [Requirements CapabilityStatement](http://hl7.org/fhir/capabilitystatement.html#requirements) describing what capabilities are potentially relevant.  It can be used as a template for creating an [Instance CapabilityStatement](http://hl7.org/fhir/capabilitystatement.html#instance) by removing expectation extensions and making actual assertions associated with each capability to describe the capabilities of a deployed and configured implementation.
-</t>
   </si>
   <si>
     <t>The Client **MAY** support transaction interactions to Getting Additional Data About Group Members</t>
@@ -581,6 +567,20 @@
   </si>
   <si>
     <t xml:space="preserve"> for fetching associated data about group members represented in the QuestionnaireResponse resource. The Client **MAY** use with comma-separated values.</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This CapabilityStatement outlines the conformance requirements and expectations for Argonaut User Facing Patient List **Client applications**.  It identifies the specific profiles and RESTful transactions for  requesting user facing patient list data from an EHR using the Argonaut User Facing Patient List API.  This includes the following interactions:
+1. Discovery of User Facing Patient Lists
+2. Fetching User Facing Patient Lists
+3. Fetching Additional Data about each Patient in a User Facing Patient Lists
+This is a [Requirements CapabilityStatement](http://hl7.org/fhir/capabilitystatement.html#requirements) describing what capabilities are potentially relevant.  It can be used as a template for creating an [Instance CapabilityStatement](http://hl7.org/fhir/capabilitystatement.html#instance) by removing expectation extensions and making actual assertions associated with each capability to describe the capabilities of a deployed and configured implementation.
+</t>
+  </si>
+  <si>
+    <t>http://www.fhir.org/guides/argonaut/patient-list/</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FE7B3C-655A-420A-A582-37B1D34DD578}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1089,7 +1089,7 @@
         <v>82</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1098,7 +1098,7 @@
         <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1106,7 +1106,7 @@
         <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
         <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1122,7 +1122,7 @@
         <v>86</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1138,7 +1138,7 @@
         <v>89</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1208,16 +1208,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -1351,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1382,7 +1382,7 @@
         <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1398,7 +1398,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1406,7 +1406,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1422,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1430,7 +1430,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1469,13 +1469,13 @@
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
@@ -1519,62 +1519,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1712,60 +1712,60 @@
     </row>
     <row r="2" spans="1:25" ht="34" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="128" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="22:25" ht="18" x14ac:dyDescent="0.2">
@@ -1857,34 +1857,34 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1919,7 +1919,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>54</v>
@@ -2140,30 +2140,30 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>26</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>26</v>
@@ -2190,7 +2190,7 @@
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2315,7 +2315,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -2327,16 +2327,16 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
@@ -2347,10 +2347,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>54</v>
@@ -2359,16 +2359,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
@@ -2379,10 +2379,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>54</v>
@@ -2391,16 +2391,16 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA4" s="5"/>
       <c r="AB4" s="11"/>
@@ -2410,10 +2410,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>54</v>
@@ -2422,16 +2422,16 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA5" s="6"/>
       <c r="AB5" s="11"/>
@@ -2441,10 +2441,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>54</v>
@@ -2453,16 +2453,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA6" s="6"/>
       <c r="AB6" s="11"/>
@@ -2472,10 +2472,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>54</v>
@@ -2484,16 +2484,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA7" s="6"/>
       <c r="AB7" s="11"/>
@@ -2503,10 +2503,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>54</v>
@@ -2515,16 +2515,16 @@
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA8" s="6"/>
       <c r="AB8" s="11"/>
@@ -2534,10 +2534,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>54</v>
@@ -2546,16 +2546,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA9" s="6"/>
       <c r="AB9" s="11"/>
@@ -2565,10 +2565,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>54</v>
@@ -2577,16 +2577,16 @@
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA10" s="6"/>
       <c r="AB10" s="11"/>
@@ -2596,10 +2596,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>54</v>
@@ -2608,16 +2608,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA11" s="6"/>
       <c r="AB11" s="11"/>
@@ -2627,10 +2627,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
@@ -2639,16 +2639,16 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA12" s="6"/>
       <c r="AB12" s="11"/>

</xml_diff>

<commit_message>
fix errors and update CapabilityStatement
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/client.xlsx
+++ b/input/resources-spreadsheet/client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Argo-PL/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55109704-AFC1-A94A-B7AE-453BC6B910AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CB7097-3294-7642-90D6-7FBFA8EA8608}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-720" windowWidth="25600" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="-720" windowWidth="25600" windowHeight="20480" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="163">
   <si>
     <t>Element</t>
   </si>
@@ -581,6 +581,9 @@
   </si>
   <si>
     <t>http://www.fhir.org/guides/argonaut/patient-list/</t>
+  </si>
+  <si>
+    <t>reference</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FE7B3C-655A-420A-A582-37B1D34DD578}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2186,11 +2189,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2400,7 +2403,7 @@
         <v>115</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="AA4" s="5"/>
       <c r="AB4" s="11"/>
@@ -2462,7 +2465,7 @@
         <v>115</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="AA6" s="6"/>
       <c r="AB6" s="11"/>

</xml_diff>